<commit_message>
Lista de picos actualizada. Migracion de DB
</commit_message>
<xml_diff>
--- a/doc/nozzles.xlsx
+++ b/doc/nozzles.xlsx
@@ -217,10 +217,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -709,7 +706,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" topLeftCell="C46" zoomScale="100" workbookViewId="0">
       <selection activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -731,13 +728,13 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1">
@@ -772,10 +769,10 @@
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>2</v>
       </c>
       <c r="C2" t="s">
@@ -784,10 +781,10 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
@@ -822,10 +819,10 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="2">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -834,10 +831,10 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G3" t="s">
@@ -872,22 +869,22 @@
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="2">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
@@ -922,22 +919,22 @@
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="2">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G5" t="s">
@@ -972,10 +969,10 @@
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="2">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" t="s">
@@ -984,10 +981,10 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G6" t="s">
@@ -1022,10 +1019,10 @@
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="2">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" t="s">
@@ -1034,10 +1031,10 @@
       <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G7" t="s">
@@ -1072,7 +1069,7 @@
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>0</v>
       </c>
       <c r="B8">
@@ -1081,13 +1078,13 @@
       <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G8" t="s">
@@ -1122,7 +1119,7 @@
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>0</v>
       </c>
       <c r="B9">
@@ -1131,13 +1128,13 @@
       <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G9" t="s">
@@ -1172,7 +1169,7 @@
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>0</v>
       </c>
       <c r="B10">
@@ -1181,13 +1178,13 @@
       <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G10" t="s">
@@ -1222,7 +1219,7 @@
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>0</v>
       </c>
       <c r="B11">
@@ -1231,13 +1228,13 @@
       <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G11" t="s">
@@ -1272,7 +1269,7 @@
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>0</v>
       </c>
       <c r="B12">
@@ -1281,13 +1278,13 @@
       <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G12" t="s">
@@ -1322,22 +1319,22 @@
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="2">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
         <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G13" t="s">
@@ -1372,7 +1369,7 @@
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>0</v>
       </c>
       <c r="B14">
@@ -1381,13 +1378,13 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G14" t="s">
@@ -1422,7 +1419,7 @@
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>0</v>
       </c>
       <c r="B15">
@@ -1431,13 +1428,13 @@
       <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G15" t="s">
@@ -1472,7 +1469,7 @@
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>0</v>
       </c>
       <c r="B16">
@@ -1481,13 +1478,13 @@
       <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G16" t="s">
@@ -1522,7 +1519,7 @@
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>0</v>
       </c>
       <c r="B17">
@@ -1531,13 +1528,13 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G17" t="s">
@@ -1572,7 +1569,7 @@
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>0</v>
       </c>
       <c r="B18">
@@ -1581,13 +1578,13 @@
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G18" t="s">
@@ -1622,7 +1619,7 @@
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>0</v>
       </c>
       <c r="B19">
@@ -1631,13 +1628,13 @@
       <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G19" t="s">
@@ -1672,7 +1669,7 @@
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>0</v>
       </c>
       <c r="B20">
@@ -1681,13 +1678,13 @@
       <c r="C20" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G20" t="s">
@@ -1722,7 +1719,7 @@
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>0</v>
       </c>
       <c r="B21">
@@ -1731,13 +1728,13 @@
       <c r="C21" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G21" t="s">
@@ -1772,7 +1769,7 @@
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>0</v>
       </c>
       <c r="B22">
@@ -1781,13 +1778,13 @@
       <c r="C22" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G22" t="s">
@@ -1822,7 +1819,7 @@
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>0</v>
       </c>
       <c r="B23">
@@ -1831,13 +1828,13 @@
       <c r="C23" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G23" t="s">
@@ -1872,22 +1869,22 @@
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="2">
-        <v>0</v>
-      </c>
-      <c r="B24" s="2">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1">
         <v>5</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G24" t="s">
@@ -1922,7 +1919,7 @@
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>0</v>
       </c>
       <c r="B25">
@@ -1931,13 +1928,13 @@
       <c r="C25" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G25" t="s">
@@ -1972,7 +1969,7 @@
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>0</v>
       </c>
       <c r="B26">
@@ -1981,13 +1978,13 @@
       <c r="C26" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G26" t="s">
@@ -2022,7 +2019,7 @@
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>0</v>
       </c>
       <c r="B27">
@@ -2031,13 +2028,13 @@
       <c r="C27" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G27" t="s">
@@ -2072,7 +2069,7 @@
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>0</v>
       </c>
       <c r="B28">
@@ -2081,13 +2078,13 @@
       <c r="C28" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G28" t="s">
@@ -2122,7 +2119,7 @@
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>0</v>
       </c>
       <c r="B29">
@@ -2131,13 +2128,13 @@
       <c r="C29" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G29" t="s">
@@ -2172,7 +2169,7 @@
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>0</v>
       </c>
       <c r="B30">
@@ -2181,13 +2178,13 @@
       <c r="C30" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G30" t="s">
@@ -2222,22 +2219,22 @@
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="2">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2">
+      <c r="A31" s="1">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
         <v>6</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G31" t="s">
@@ -2272,7 +2269,7 @@
       </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>0</v>
       </c>
       <c r="B32">
@@ -2281,13 +2278,13 @@
       <c r="C32" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G32" t="s">
@@ -2322,7 +2319,7 @@
       </c>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>0</v>
       </c>
       <c r="B33">
@@ -2331,13 +2328,13 @@
       <c r="C33" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G33" t="s">
@@ -2372,7 +2369,7 @@
       </c>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>0</v>
       </c>
       <c r="B34">
@@ -2381,13 +2378,13 @@
       <c r="C34" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G34" t="s">
@@ -2422,7 +2419,7 @@
       </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>0</v>
       </c>
       <c r="B35">
@@ -2431,13 +2428,13 @@
       <c r="C35" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G35" t="s">
@@ -2472,7 +2469,7 @@
       </c>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>0</v>
       </c>
       <c r="B36">
@@ -2481,13 +2478,13 @@
       <c r="C36" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G36" t="s">
@@ -2522,7 +2519,7 @@
       </c>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>0</v>
       </c>
       <c r="B37">
@@ -2531,13 +2528,13 @@
       <c r="C37" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G37" t="s">
@@ -2572,7 +2569,7 @@
       </c>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>0</v>
       </c>
       <c r="B38">
@@ -2581,13 +2578,13 @@
       <c r="C38" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G38" t="s">
@@ -2622,7 +2619,7 @@
       </c>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>0</v>
       </c>
       <c r="B39">
@@ -2631,13 +2628,13 @@
       <c r="C39" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G39" t="s">
@@ -2672,7 +2669,7 @@
       </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>0</v>
       </c>
       <c r="B40">
@@ -2681,13 +2678,13 @@
       <c r="C40" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G40" t="s">
@@ -2722,7 +2719,7 @@
       </c>
     </row>
     <row r="41" ht="14.25">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>0</v>
       </c>
       <c r="B41">
@@ -2731,13 +2728,13 @@
       <c r="C41" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G41" t="s">
@@ -2772,22 +2769,22 @@
       </c>
     </row>
     <row r="42" ht="14.25">
-      <c r="A42" s="2">
-        <v>0</v>
-      </c>
-      <c r="B42" s="2">
+      <c r="A42" s="1">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1">
         <v>7</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G42" t="s">
@@ -2822,7 +2819,7 @@
       </c>
     </row>
     <row r="43" ht="14.25">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>0</v>
       </c>
       <c r="B43">
@@ -2831,13 +2828,13 @@
       <c r="C43" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G43" t="s">
@@ -2872,7 +2869,7 @@
       </c>
     </row>
     <row r="44" ht="14.25">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>0</v>
       </c>
       <c r="B44">
@@ -2881,13 +2878,13 @@
       <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G44" t="s">
@@ -2922,7 +2919,7 @@
       </c>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>0</v>
       </c>
       <c r="B45">
@@ -2931,13 +2928,13 @@
       <c r="C45" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G45" t="s">
@@ -2972,7 +2969,7 @@
       </c>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>0</v>
       </c>
       <c r="B46">
@@ -2981,13 +2978,13 @@
       <c r="C46" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G46" t="s">
@@ -3022,7 +3019,7 @@
       </c>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>0</v>
       </c>
       <c r="B47">
@@ -3031,13 +3028,13 @@
       <c r="C47" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F47" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G47" t="s">
@@ -3072,7 +3069,7 @@
       </c>
     </row>
     <row r="48" ht="14.25">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>0</v>
       </c>
       <c r="B48">
@@ -3081,13 +3078,13 @@
       <c r="C48" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G48" t="s">
@@ -3122,7 +3119,7 @@
       </c>
     </row>
     <row r="49" ht="14.25">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>0</v>
       </c>
       <c r="B49">
@@ -3131,13 +3128,13 @@
       <c r="C49" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G49" t="s">
@@ -3172,7 +3169,7 @@
       </c>
     </row>
     <row r="50" ht="14.25">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>0</v>
       </c>
       <c r="B50">
@@ -3181,13 +3178,13 @@
       <c r="C50" t="s">
         <v>34</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G50" t="s">
@@ -3222,7 +3219,7 @@
       </c>
     </row>
     <row r="51" ht="14.25">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>0</v>
       </c>
       <c r="B51">
@@ -3231,13 +3228,13 @@
       <c r="C51" t="s">
         <v>37</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F51" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G51" t="s">
@@ -3272,7 +3269,7 @@
       </c>
     </row>
     <row r="52" ht="14.25">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>0</v>
       </c>
       <c r="B52">
@@ -3281,13 +3278,13 @@
       <c r="C52" t="s">
         <v>41</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G52" t="s">
@@ -3322,22 +3319,22 @@
       </c>
     </row>
     <row r="53" ht="14.25">
-      <c r="A53" s="2">
-        <v>0</v>
-      </c>
-      <c r="B53" s="2">
+      <c r="A53" s="1">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1">
         <v>8</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E53" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G53" t="s">
@@ -3372,7 +3369,7 @@
       </c>
     </row>
     <row r="54" ht="14.25">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>0</v>
       </c>
       <c r="B54">
@@ -3381,13 +3378,13 @@
       <c r="C54" t="s">
         <v>13</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F54" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G54" t="s">
@@ -3422,7 +3419,7 @@
       </c>
     </row>
     <row r="55" ht="14.25">
-      <c r="A55" s="2">
+      <c r="A55" s="1">
         <v>0</v>
       </c>
       <c r="B55">
@@ -3431,13 +3428,13 @@
       <c r="C55" t="s">
         <v>44</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G55" t="s">
@@ -3472,7 +3469,7 @@
       </c>
     </row>
     <row r="56" ht="14.25">
-      <c r="A56" s="2">
+      <c r="A56" s="1">
         <v>0</v>
       </c>
       <c r="B56">
@@ -3481,13 +3478,13 @@
       <c r="C56" t="s">
         <v>48</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F56" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G56" t="s">
@@ -3522,7 +3519,7 @@
       </c>
     </row>
     <row r="57" ht="14.25">
-      <c r="A57" s="2">
+      <c r="A57" s="1">
         <v>0</v>
       </c>
       <c r="B57">
@@ -3531,13 +3528,13 @@
       <c r="C57" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F57" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G57" t="s">
@@ -3572,7 +3569,7 @@
       </c>
     </row>
     <row r="58" ht="14.25">
-      <c r="A58" s="2">
+      <c r="A58" s="1">
         <v>0</v>
       </c>
       <c r="B58">
@@ -3581,13 +3578,13 @@
       <c r="C58" t="s">
         <v>24</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F58" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G58" t="s">
@@ -3622,7 +3619,7 @@
       </c>
     </row>
     <row r="59" ht="14.25">
-      <c r="A59" s="2">
+      <c r="A59" s="1">
         <v>0</v>
       </c>
       <c r="B59">
@@ -3631,13 +3628,13 @@
       <c r="C59" t="s">
         <v>26</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F59" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G59" t="s">
@@ -3672,7 +3669,7 @@
       </c>
     </row>
     <row r="60" ht="14.25">
-      <c r="A60" s="2">
+      <c r="A60" s="1">
         <v>0</v>
       </c>
       <c r="B60">
@@ -3681,13 +3678,13 @@
       <c r="C60" t="s">
         <v>30</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G60" t="s">
@@ -3722,7 +3719,7 @@
       </c>
     </row>
     <row r="61" ht="14.25">
-      <c r="A61" s="2">
+      <c r="A61" s="1">
         <v>0</v>
       </c>
       <c r="B61">
@@ -3731,13 +3728,13 @@
       <c r="C61" t="s">
         <v>34</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F61" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G61" t="s">
@@ -3772,7 +3769,7 @@
       </c>
     </row>
     <row r="62" ht="14.25">
-      <c r="A62" s="2">
+      <c r="A62" s="1">
         <v>0</v>
       </c>
       <c r="B62">
@@ -3781,13 +3778,13 @@
       <c r="C62" t="s">
         <v>37</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F62" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G62" t="s">
@@ -3822,7 +3819,7 @@
       </c>
     </row>
     <row r="63" ht="14.25">
-      <c r="A63" s="2">
+      <c r="A63" s="1">
         <v>0</v>
       </c>
       <c r="B63">
@@ -3831,13 +3828,13 @@
       <c r="C63" t="s">
         <v>41</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F63" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G63" t="s">
@@ -3872,22 +3869,22 @@
       </c>
     </row>
     <row r="64" ht="14.25">
-      <c r="A64" s="2">
-        <v>0</v>
-      </c>
-      <c r="B64" s="2">
+      <c r="A64" s="1">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1">
         <v>9</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E64" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F64" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G64" t="s">
@@ -3922,7 +3919,7 @@
       </c>
     </row>
     <row r="65" ht="14.25">
-      <c r="A65" s="2">
+      <c r="A65" s="1">
         <v>0</v>
       </c>
       <c r="B65">
@@ -3931,13 +3928,13 @@
       <c r="C65" t="s">
         <v>13</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G65" t="s">
@@ -3972,7 +3969,7 @@
       </c>
     </row>
     <row r="66" ht="14.25">
-      <c r="A66" s="2">
+      <c r="A66" s="1">
         <v>0</v>
       </c>
       <c r="B66">
@@ -3981,13 +3978,13 @@
       <c r="C66" t="s">
         <v>44</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G66" t="s">
@@ -4022,7 +4019,7 @@
       </c>
     </row>
     <row r="67" ht="14.25">
-      <c r="A67" s="2">
+      <c r="A67" s="1">
         <v>0</v>
       </c>
       <c r="B67">
@@ -4031,13 +4028,13 @@
       <c r="C67" t="s">
         <v>48</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F67" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G67" t="s">
@@ -4072,7 +4069,7 @@
       </c>
     </row>
     <row r="68" ht="14.25">
-      <c r="A68" s="2">
+      <c r="A68" s="1">
         <v>0</v>
       </c>
       <c r="B68">
@@ -4081,13 +4078,13 @@
       <c r="C68" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="F68" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G68" t="s">
@@ -4122,7 +4119,7 @@
       </c>
     </row>
     <row r="69" ht="14.25">
-      <c r="A69" s="2">
+      <c r="A69" s="1">
         <v>0</v>
       </c>
       <c r="B69">
@@ -4131,13 +4128,13 @@
       <c r="C69" t="s">
         <v>24</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="F69" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G69" t="s">
@@ -4172,7 +4169,7 @@
       </c>
     </row>
     <row r="70" ht="14.25">
-      <c r="A70" s="2">
+      <c r="A70" s="1">
         <v>0</v>
       </c>
       <c r="B70">
@@ -4181,26 +4178,26 @@
       <c r="C70" t="s">
         <v>26</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="F70" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G70" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H70" t="s">
         <v>19</v>
       </c>
       <c r="I70" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J70" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K70" t="s">
         <v>19</v>
@@ -4222,7 +4219,7 @@
       </c>
     </row>
     <row r="71" ht="14.25">
-      <c r="A71" s="2">
+      <c r="A71" s="1">
         <v>0</v>
       </c>
       <c r="B71">
@@ -4231,13 +4228,13 @@
       <c r="C71" t="s">
         <v>37</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="F71" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G71" t="s">

</xml_diff>

<commit_message>
Estilo selectores de picos. Correcciones formulario parametros
</commit_message>
<xml_diff>
--- a/doc/nozzles.xlsx
+++ b/doc/nozzles.xlsx
@@ -706,16 +706,18 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" topLeftCell="C46" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" view="normal" zoomScale="100" workbookViewId="0">
       <selection activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" style="0" width="14.710000000000001"/>
-    <col customWidth="1" min="3" max="4" style="0" width="11.85"/>
-    <col customWidth="1" min="5" max="5" style="0" width="36.280000000000001"/>
-    <col customWidth="1" min="6" max="6" style="0" width="17.57"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="0" width="6.57421875"/>
+    <col customWidth="1" min="2" max="2" style="0" width="6.7109375"/>
+    <col customWidth="1" min="3" max="3" style="0" width="11.85"/>
+    <col customWidth="1" min="4" max="4" style="0" width="9.7109375"/>
+    <col customWidth="1" min="5" max="5" style="0" width="15.421875"/>
+    <col customWidth="1" min="6" max="6" style="0" width="6.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">

</xml_diff>